<commit_message>
Major changes on analysis code, figures, etc. in response to observations by peer reviewers.
</commit_message>
<xml_diff>
--- a/data/dictionary_atelectasis_prevalence.xlsx
+++ b/data/dictionary_atelectasis_prevalence.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://comunidadunammx-my.sharepoint.com/personal/javimangal_comunidad_unam_mx/Documents/Mancilla-Kammar Lab/Tesis/Manuel Guerrero/Atelectasias/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\javim\Documents\GitHub\preoperative-atelectasis\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="288" documentId="8_{45809E0E-C229-48F0-8CAD-D38185A39F16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{51AF5B14-ED56-4D28-9720-3EA661BC5C87}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{691ABC4A-F0DE-462F-B79F-0EDE509B5995}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-15735" yWindow="-16320" windowWidth="29040" windowHeight="15720" xr2:uid="{4450A967-A323-479D-A643-59738EE9059C}"/>
+    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{4450A967-A323-479D-A643-59738EE9059C}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="320" uniqueCount="185">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="362" uniqueCount="203">
   <si>
     <t>Variable</t>
   </si>
@@ -330,9 +330,6 @@
     <t xml:space="preserve">Biological sex as registered in medical records. </t>
   </si>
   <si>
-    <t>Medical history of systemic arterial hypertension according to medical records.</t>
-  </si>
-  <si>
     <t>0 = "No", 1 = "Yes"</t>
   </si>
   <si>
@@ -420,15 +417,6 @@
     <t xml:space="preserve">The upper limit for allowed values given here is arbitrary and is only shown to give an idea of a range of possible values, since no restrictions for surgery exist upon an uper limit of BMI at our center. </t>
   </si>
   <si>
-    <t>Presence of at least one additional comorbidity according to medical records.</t>
-  </si>
-  <si>
-    <t>Medical history of obstructive sleep apnea according to medical records.</t>
-  </si>
-  <si>
-    <t>Medical history of hypothiroidism according to medical records.</t>
-  </si>
-  <si>
     <t>cells/µL</t>
   </si>
   <si>
@@ -498,9 +486,6 @@
     <t>Obstructive sleep apnea</t>
   </si>
   <si>
-    <t>Medical history of diabetes mellitus according to medical records.</t>
-  </si>
-  <si>
     <t>Diabetes mellitus</t>
   </si>
   <si>
@@ -513,15 +498,6 @@
     <t>Other comorbidities</t>
   </si>
   <si>
-    <t>Medical history of dyslipidemia according to medical records.</t>
-  </si>
-  <si>
-    <t>Medical history of use of antidepressants according to medical records.</t>
-  </si>
-  <si>
-    <t>Medical history of prior COVID-19 according to medical records.</t>
-  </si>
-  <si>
     <t>0.00-100.00</t>
   </si>
   <si>
@@ -604,6 +580,84 @@
   </si>
   <si>
     <t xml:space="preserve">Upon arrival at the hospital, a rapid SARS-CoV-2 antibody testing was performed. If IgM against SARS-CoV-2 was positive, the surgery was postponed. ) If the antibody test was negative, a chest computed tomography (CT) was performed and a CO-RADS4 score ≥3 was considered suggestive of COVID-19, leading to cancellation of the surgery. We were not able to recover the details of the specific test applied to give information on the target SARS-CoV-2 subunits antibodies nor the sensitivity or specificity of the test. </t>
+  </si>
+  <si>
+    <t>myocardial_infarction</t>
+  </si>
+  <si>
+    <t>tuberculosis</t>
+  </si>
+  <si>
+    <t>asthma</t>
+  </si>
+  <si>
+    <t>COPD</t>
+  </si>
+  <si>
+    <t>oxygen_use</t>
+  </si>
+  <si>
+    <t>CPAP_use</t>
+  </si>
+  <si>
+    <t>Tuberculosis</t>
+  </si>
+  <si>
+    <t>Asthma</t>
+  </si>
+  <si>
+    <t>Acute myocardial infarction</t>
+  </si>
+  <si>
+    <t>Chronic obstructive pulmonary disease</t>
+  </si>
+  <si>
+    <t>Use of supplementary oxygen therapy at home</t>
+  </si>
+  <si>
+    <t>Continuous positive airway pressure therapy at home</t>
+  </si>
+  <si>
+    <t>Medical history of prior COVID-19 according to medical records or self-report questionnaire.</t>
+  </si>
+  <si>
+    <t>Medical history of use of antidepressants according to medical records or self-report questionnaire.</t>
+  </si>
+  <si>
+    <t>Presence of at least one additional comorbidity according to medical records or self-report questionnaire.</t>
+  </si>
+  <si>
+    <t>Medical history of dyslipidemia according to medical records or self-report questionnaire.</t>
+  </si>
+  <si>
+    <t>Medical history of hypothiroidism according to medical records or self-report questionnaire.</t>
+  </si>
+  <si>
+    <t>Medical history of diabetes mellitus according to medical records or self-report questionnaire.</t>
+  </si>
+  <si>
+    <t>Medical history of systemic arterial hypertension according to medical records or self-report questionnaire.</t>
+  </si>
+  <si>
+    <t>Medical history of obstructive sleep apnea according to medical records or self-report questionnaire.</t>
+  </si>
+  <si>
+    <t>Medical history of continuous positive airway pressure (CPAP) therapy at home according to medical records or self-report questionnaire.</t>
+  </si>
+  <si>
+    <t>Medical history of acute myocardial infarction according to medical records or self-report questionnaire.</t>
+  </si>
+  <si>
+    <t>Medical history of tuberculosis according to medical records or self-report questionnaire.</t>
+  </si>
+  <si>
+    <t>Medical history of asthma according to medical records or self-report questionnaire.</t>
+  </si>
+  <si>
+    <t>Medical history of chronic obstructive pulmonary disease (COPD) according to medical records or self-report questionnaire.</t>
+  </si>
+  <si>
+    <t>Medical history of supplementary oxygen therapy at home according to medical records or self-report questionnaire.</t>
   </si>
 </sst>
 </file>
@@ -670,11 +724,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -682,10 +735,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -708,9 +761,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - Tema de 2022">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -748,7 +801,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -854,7 +907,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -996,7 +1049,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1004,17 +1057,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D03469C4-704E-4F14-9796-1296DD372ECF}">
-  <dimension ref="A1:I43"/>
+  <dimension ref="A1:I49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F11" sqref="F11"/>
+      <selection pane="bottomLeft" activeCell="G40" sqref="G40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.21875" style="6" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.88671875" customWidth="1"/>
+    <col min="2" max="2" width="19.5546875" style="5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17.109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="32.6640625" customWidth="1"/>
     <col min="5" max="5" width="18" customWidth="1"/>
@@ -1026,7 +1079,7 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
@@ -1048,14 +1101,14 @@
         <v>74</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>47</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="4" t="s">
         <v>5</v>
       </c>
       <c r="C2" t="s">
@@ -1078,7 +1131,7 @@
       <c r="A3" t="s">
         <v>49</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="4" t="s">
         <v>6</v>
       </c>
       <c r="C3" t="s">
@@ -1104,7 +1157,7 @@
       <c r="A4" t="s">
         <v>51</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="4" t="s">
         <v>7</v>
       </c>
       <c r="C4" t="s">
@@ -1130,7 +1183,7 @@
       <c r="A5" t="s">
         <v>61</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="4" t="s">
         <v>8</v>
       </c>
       <c r="C5" t="s">
@@ -1143,20 +1196,20 @@
         <v>66</v>
       </c>
       <c r="G5" t="s">
-        <v>167</v>
-      </c>
-      <c r="H5" s="4" t="s">
-        <v>177</v>
+        <v>159</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>169</v>
       </c>
       <c r="I5" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>62</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="4" t="s">
         <v>9</v>
       </c>
       <c r="C6" t="s">
@@ -1169,17 +1222,17 @@
         <v>67</v>
       </c>
       <c r="G6" t="s">
-        <v>168</v>
+        <v>160</v>
       </c>
       <c r="I6" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="16.2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>63</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="4" t="s">
         <v>10</v>
       </c>
       <c r="C7" t="s">
@@ -1192,38 +1245,38 @@
         <v>68</v>
       </c>
       <c r="G7" t="s">
-        <v>169</v>
-      </c>
-      <c r="H7" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="H7" s="3" t="s">
         <v>75</v>
       </c>
       <c r="I7" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>70</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="B8" s="4" t="s">
         <v>11</v>
       </c>
       <c r="C8" t="s">
         <v>60</v>
       </c>
-      <c r="D8" s="3" t="s">
+      <c r="D8" t="s">
         <v>71</v>
       </c>
-      <c r="E8" s="3" t="s">
+      <c r="E8" t="s">
         <v>73</v>
       </c>
       <c r="F8" t="s">
         <v>72</v>
       </c>
       <c r="G8" t="s">
-        <v>170</v>
-      </c>
-      <c r="H8" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="H8" s="3" t="s">
         <v>75</v>
       </c>
     </row>
@@ -1231,118 +1284,118 @@
       <c r="A9" t="s">
         <v>77</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="B9" s="4" t="s">
         <v>12</v>
       </c>
       <c r="C9" t="s">
         <v>50</v>
       </c>
-      <c r="D9" s="3" t="s">
+      <c r="D9" t="s">
+        <v>114</v>
+      </c>
+      <c r="E9" t="s">
         <v>115</v>
       </c>
-      <c r="E9" t="s">
-        <v>116</v>
-      </c>
       <c r="G9" t="s">
-        <v>171</v>
-      </c>
-      <c r="H9" s="4" t="s">
-        <v>95</v>
+        <v>163</v>
+      </c>
+      <c r="H9" s="3" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>78</v>
       </c>
-      <c r="B10" s="5" t="s">
+      <c r="B10" s="4" t="s">
         <v>13</v>
       </c>
       <c r="C10" t="s">
         <v>60</v>
       </c>
-      <c r="D10" s="3" t="s">
-        <v>114</v>
-      </c>
-      <c r="E10" s="3" t="s">
+      <c r="D10" t="s">
+        <v>113</v>
+      </c>
+      <c r="E10" t="s">
         <v>73</v>
       </c>
       <c r="G10" t="s">
-        <v>172</v>
-      </c>
-      <c r="H10" s="4" t="s">
-        <v>95</v>
+        <v>164</v>
+      </c>
+      <c r="H10" s="3" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>88</v>
       </c>
-      <c r="B11" s="5" t="s">
+      <c r="B11" s="4" t="s">
         <v>14</v>
       </c>
       <c r="C11" t="s">
         <v>60</v>
       </c>
-      <c r="D11" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="E11" s="3" t="s">
+      <c r="D11" t="s">
+        <v>99</v>
+      </c>
+      <c r="E11" t="s">
         <v>73</v>
       </c>
       <c r="G11" t="s">
-        <v>96</v>
-      </c>
-      <c r="H11" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="H11" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="I11" t="s">
         <v>98</v>
-      </c>
-      <c r="I11" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>76</v>
       </c>
-      <c r="B12" s="5" t="s">
+      <c r="B12" s="4" t="s">
         <v>15</v>
       </c>
       <c r="C12" t="s">
         <v>50</v>
       </c>
-      <c r="D12" s="3" t="s">
-        <v>173</v>
+      <c r="D12" t="s">
+        <v>165</v>
       </c>
       <c r="E12" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F12" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G12" t="s">
-        <v>174</v>
-      </c>
-      <c r="H12" s="4" t="s">
-        <v>178</v>
+        <v>166</v>
+      </c>
+      <c r="H12" s="3" t="s">
+        <v>170</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>84</v>
       </c>
-      <c r="B13" s="5" t="s">
+      <c r="B13" s="4" t="s">
         <v>16</v>
       </c>
       <c r="C13" t="s">
         <v>60</v>
       </c>
-      <c r="D13" s="3" t="s">
+      <c r="D13" t="s">
         <v>83</v>
       </c>
       <c r="E13" t="s">
         <v>73</v>
       </c>
       <c r="G13" t="s">
-        <v>180</v>
+        <v>172</v>
       </c>
       <c r="H13" t="s">
         <v>73</v>
@@ -1352,13 +1405,13 @@
       <c r="A14" t="s">
         <v>87</v>
       </c>
-      <c r="B14" s="5" t="s">
+      <c r="B14" s="4" t="s">
         <v>17</v>
       </c>
       <c r="C14" t="s">
         <v>60</v>
       </c>
-      <c r="D14" s="3" t="s">
+      <c r="D14" t="s">
         <v>90</v>
       </c>
       <c r="E14" t="s">
@@ -1367,7 +1420,7 @@
       <c r="G14" t="s">
         <v>91</v>
       </c>
-      <c r="H14" s="4" t="s">
+      <c r="H14" s="3" t="s">
         <v>89</v>
       </c>
     </row>
@@ -1375,208 +1428,208 @@
       <c r="A15" t="s">
         <v>52</v>
       </c>
-      <c r="B15" s="5" t="s">
+      <c r="B15" s="4" t="s">
         <v>18</v>
       </c>
       <c r="C15" t="s">
         <v>60</v>
       </c>
-      <c r="D15" s="3" t="s">
-        <v>94</v>
+      <c r="D15" t="s">
+        <v>93</v>
       </c>
       <c r="E15" t="s">
         <v>73</v>
       </c>
       <c r="G15" s="7" t="s">
-        <v>175</v>
-      </c>
-      <c r="H15" s="9" t="s">
-        <v>179</v>
+        <v>167</v>
+      </c>
+      <c r="H15" s="8" t="s">
+        <v>171</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>85</v>
       </c>
-      <c r="B16" s="5" t="s">
+      <c r="B16" s="4" t="s">
         <v>19</v>
       </c>
       <c r="C16" t="s">
         <v>60</v>
       </c>
-      <c r="D16" s="3" t="s">
-        <v>102</v>
+      <c r="D16" t="s">
+        <v>101</v>
       </c>
       <c r="E16" t="s">
         <v>73</v>
       </c>
       <c r="G16" s="7"/>
-      <c r="H16" s="9"/>
+      <c r="H16" s="8"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>86</v>
       </c>
-      <c r="B17" s="5" t="s">
+      <c r="B17" s="4" t="s">
         <v>20</v>
       </c>
       <c r="C17" t="s">
         <v>50</v>
       </c>
-      <c r="D17" s="3" t="s">
-        <v>113</v>
+      <c r="D17" t="s">
+        <v>112</v>
       </c>
       <c r="E17" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G17" s="7"/>
-      <c r="H17" s="9"/>
+      <c r="H17" s="8"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>103</v>
-      </c>
-      <c r="B18" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="B18" s="4" t="s">
         <v>21</v>
       </c>
       <c r="C18" t="s">
         <v>50</v>
       </c>
-      <c r="D18" s="3" t="s">
+      <c r="D18" t="s">
+        <v>117</v>
+      </c>
+      <c r="E18" t="s">
+        <v>103</v>
+      </c>
+      <c r="G18" t="s">
+        <v>168</v>
+      </c>
+      <c r="H18" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="I18" t="s">
         <v>118</v>
-      </c>
-      <c r="E18" t="s">
-        <v>104</v>
-      </c>
-      <c r="G18" t="s">
-        <v>176</v>
-      </c>
-      <c r="H18" s="4" t="s">
-        <v>117</v>
-      </c>
-      <c r="I18" t="s">
-        <v>119</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>112</v>
-      </c>
-      <c r="B19" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="B19" s="4" t="s">
         <v>22</v>
       </c>
       <c r="C19" t="s">
         <v>50</v>
       </c>
-      <c r="D19" s="3" t="s">
-        <v>157</v>
+      <c r="D19" t="s">
+        <v>149</v>
       </c>
       <c r="E19" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G19" t="s">
-        <v>176</v>
-      </c>
-      <c r="H19" s="4" t="s">
-        <v>117</v>
+        <v>168</v>
+      </c>
+      <c r="H19" s="3" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>111</v>
-      </c>
-      <c r="B20" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="B20" s="4" t="s">
         <v>23</v>
       </c>
       <c r="C20" t="s">
         <v>50</v>
       </c>
-      <c r="D20" s="3" t="s">
-        <v>158</v>
+      <c r="D20" t="s">
+        <v>150</v>
       </c>
       <c r="E20" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F20" t="s">
-        <v>164</v>
+        <v>156</v>
       </c>
       <c r="G20" t="s">
-        <v>176</v>
-      </c>
-      <c r="H20" s="8" t="s">
+        <v>168</v>
+      </c>
+      <c r="H20" s="6" t="s">
         <v>73</v>
       </c>
       <c r="I20" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>107</v>
-      </c>
-      <c r="B21" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="B21" s="4" t="s">
         <v>24</v>
       </c>
       <c r="C21" t="s">
         <v>50</v>
       </c>
-      <c r="D21" s="3" t="s">
-        <v>157</v>
+      <c r="D21" t="s">
+        <v>149</v>
       </c>
       <c r="E21" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G21" t="s">
-        <v>176</v>
-      </c>
-      <c r="H21" s="8" t="s">
+        <v>168</v>
+      </c>
+      <c r="H21" s="6" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>108</v>
-      </c>
-      <c r="B22" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="B22" s="4" t="s">
         <v>25</v>
       </c>
       <c r="C22" t="s">
         <v>50</v>
       </c>
-      <c r="D22" s="3" t="s">
-        <v>158</v>
+      <c r="D22" t="s">
+        <v>150</v>
       </c>
       <c r="E22" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="G22" t="s">
-        <v>176</v>
-      </c>
-      <c r="H22" s="8" t="s">
+        <v>168</v>
+      </c>
+      <c r="H22" s="6" t="s">
         <v>73</v>
       </c>
       <c r="I22" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>109</v>
-      </c>
-      <c r="B23" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="B23" s="4" t="s">
         <v>26</v>
       </c>
       <c r="C23" t="s">
         <v>50</v>
       </c>
-      <c r="D23" s="3" t="s">
-        <v>157</v>
+      <c r="D23" t="s">
+        <v>149</v>
       </c>
       <c r="E23" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G23" t="s">
-        <v>176</v>
+        <v>168</v>
       </c>
       <c r="H23" t="s">
         <v>73</v>
@@ -1584,48 +1637,48 @@
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>110</v>
-      </c>
-      <c r="B24" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="B24" s="4" t="s">
         <v>27</v>
       </c>
       <c r="C24" t="s">
         <v>50</v>
       </c>
-      <c r="D24" s="3" t="s">
-        <v>159</v>
+      <c r="D24" t="s">
+        <v>151</v>
       </c>
       <c r="E24" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="G24" t="s">
-        <v>176</v>
+        <v>168</v>
       </c>
       <c r="H24" t="s">
         <v>73</v>
       </c>
       <c r="I24" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>130</v>
-      </c>
-      <c r="B25" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="B25" s="4" t="s">
         <v>28</v>
       </c>
       <c r="C25" t="s">
         <v>50</v>
       </c>
-      <c r="D25" s="3" t="s">
-        <v>157</v>
+      <c r="D25" t="s">
+        <v>149</v>
       </c>
       <c r="E25" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G25" t="s">
-        <v>176</v>
+        <v>168</v>
       </c>
       <c r="H25" t="s">
         <v>73</v>
@@ -1633,204 +1686,204 @@
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>131</v>
-      </c>
-      <c r="B26" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="B26" s="4" t="s">
         <v>29</v>
       </c>
       <c r="C26" t="s">
         <v>50</v>
       </c>
-      <c r="D26" s="3" t="s">
-        <v>159</v>
+      <c r="D26" t="s">
+        <v>151</v>
       </c>
       <c r="E26" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="G26" t="s">
-        <v>176</v>
+        <v>168</v>
       </c>
       <c r="H26" t="s">
         <v>73</v>
       </c>
       <c r="I26" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>129</v>
-      </c>
-      <c r="B27" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="B27" s="4" t="s">
         <v>30</v>
       </c>
       <c r="C27" t="s">
         <v>50</v>
       </c>
-      <c r="D27" s="3" t="s">
-        <v>160</v>
+      <c r="D27" t="s">
+        <v>152</v>
       </c>
       <c r="E27" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="G27" t="s">
-        <v>176</v>
+        <v>168</v>
       </c>
       <c r="H27" t="s">
         <v>73</v>
       </c>
       <c r="I27" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>133</v>
-      </c>
-      <c r="B28" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="B28" s="4" t="s">
         <v>31</v>
       </c>
       <c r="C28" t="s">
         <v>50</v>
       </c>
-      <c r="D28" s="3" t="s">
-        <v>161</v>
+      <c r="D28" t="s">
+        <v>153</v>
       </c>
       <c r="E28" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="G28" t="s">
-        <v>176</v>
+        <v>168</v>
       </c>
       <c r="H28" t="s">
         <v>73</v>
       </c>
       <c r="I28" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>134</v>
-      </c>
-      <c r="B29" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="B29" s="4" t="s">
         <v>32</v>
       </c>
       <c r="C29" t="s">
         <v>50</v>
       </c>
-      <c r="D29" s="3" t="s">
-        <v>162</v>
+      <c r="D29" t="s">
+        <v>154</v>
       </c>
       <c r="E29" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="G29" t="s">
-        <v>176</v>
+        <v>168</v>
       </c>
       <c r="H29" t="s">
         <v>73</v>
       </c>
       <c r="I29" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>135</v>
-      </c>
-      <c r="B30" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="B30" s="4" t="s">
         <v>33</v>
       </c>
       <c r="C30" t="s">
         <v>50</v>
       </c>
-      <c r="D30" s="3" t="s">
-        <v>163</v>
+      <c r="D30" t="s">
+        <v>155</v>
       </c>
       <c r="E30" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="G30" t="s">
-        <v>176</v>
+        <v>168</v>
       </c>
       <c r="H30" t="s">
         <v>73</v>
       </c>
       <c r="I30" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>136</v>
-      </c>
-      <c r="B31" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="B31" s="4" t="s">
         <v>34</v>
       </c>
       <c r="C31" t="s">
         <v>60</v>
       </c>
-      <c r="D31" s="3" t="s">
-        <v>166</v>
+      <c r="D31" t="s">
+        <v>158</v>
       </c>
       <c r="E31" t="s">
         <v>73</v>
       </c>
       <c r="G31" t="s">
-        <v>181</v>
+        <v>173</v>
       </c>
       <c r="H31" t="s">
         <v>73</v>
       </c>
       <c r="I31" t="s">
-        <v>184</v>
+        <v>176</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>137</v>
-      </c>
-      <c r="B32" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="B32" s="4" t="s">
         <v>35</v>
       </c>
       <c r="C32" t="s">
         <v>60</v>
       </c>
-      <c r="D32" s="3" t="s">
-        <v>166</v>
+      <c r="D32" t="s">
+        <v>158</v>
       </c>
       <c r="E32" t="s">
         <v>73</v>
       </c>
       <c r="G32" t="s">
-        <v>182</v>
+        <v>174</v>
       </c>
       <c r="H32" t="s">
         <v>73</v>
       </c>
       <c r="I32" t="s">
-        <v>183</v>
+        <v>175</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>138</v>
-      </c>
-      <c r="B33" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="B33" s="4" t="s">
         <v>36</v>
       </c>
       <c r="C33" t="s">
         <v>60</v>
       </c>
-      <c r="D33" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="E33" s="3" t="s">
+      <c r="D33" t="s">
+        <v>93</v>
+      </c>
+      <c r="E33" t="s">
         <v>73</v>
       </c>
       <c r="G33" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="H33" t="s">
         <v>73</v>
@@ -1838,9 +1891,9 @@
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>165</v>
-      </c>
-      <c r="B34" s="5" t="s">
+        <v>157</v>
+      </c>
+      <c r="B34" s="4" t="s">
         <v>37</v>
       </c>
       <c r="C34" t="s">
@@ -1853,7 +1906,7 @@
         <v>73</v>
       </c>
       <c r="G34" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="H34" t="s">
         <v>73</v>
@@ -1861,51 +1914,51 @@
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>142</v>
-      </c>
-      <c r="B35" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="B35" s="4" t="s">
         <v>38</v>
       </c>
       <c r="C35" t="s">
         <v>50</v>
       </c>
       <c r="D35" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="E35" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="F35" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="G35" t="s">
-        <v>144</v>
-      </c>
-      <c r="H35" s="4" t="s">
-        <v>145</v>
+        <v>140</v>
+      </c>
+      <c r="H35" s="3" t="s">
+        <v>141</v>
       </c>
       <c r="I35" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>147</v>
-      </c>
-      <c r="B36" s="5" t="s">
-        <v>39</v>
+        <v>185</v>
+      </c>
+      <c r="B36" s="4" t="s">
+        <v>177</v>
       </c>
       <c r="C36" t="s">
         <v>60</v>
       </c>
-      <c r="D36" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="E36" s="3" t="s">
+      <c r="D36" t="s">
+        <v>93</v>
+      </c>
+      <c r="E36" t="s">
         <v>73</v>
       </c>
       <c r="G36" t="s">
-        <v>93</v>
+        <v>198</v>
       </c>
       <c r="H36" t="s">
         <v>73</v>
@@ -1913,22 +1966,22 @@
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>150</v>
-      </c>
-      <c r="B37" s="5" t="s">
-        <v>40</v>
+        <v>183</v>
+      </c>
+      <c r="B37" s="4" t="s">
+        <v>178</v>
       </c>
       <c r="C37" t="s">
         <v>60</v>
       </c>
-      <c r="D37" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="E37" s="3" t="s">
+      <c r="D37" t="s">
+        <v>93</v>
+      </c>
+      <c r="E37" t="s">
         <v>73</v>
       </c>
       <c r="G37" t="s">
-        <v>149</v>
+        <v>199</v>
       </c>
       <c r="H37" t="s">
         <v>73</v>
@@ -1936,22 +1989,22 @@
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>148</v>
-      </c>
-      <c r="B38" s="5" t="s">
-        <v>41</v>
+        <v>184</v>
+      </c>
+      <c r="B38" s="4" t="s">
+        <v>179</v>
       </c>
       <c r="C38" t="s">
         <v>60</v>
       </c>
-      <c r="D38" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="E38" s="3" t="s">
+      <c r="D38" t="s">
+        <v>93</v>
+      </c>
+      <c r="E38" t="s">
         <v>73</v>
       </c>
       <c r="G38" t="s">
-        <v>124</v>
+        <v>200</v>
       </c>
       <c r="H38" t="s">
         <v>73</v>
@@ -1959,22 +2012,22 @@
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>53</v>
-      </c>
-      <c r="B39" s="5" t="s">
-        <v>42</v>
+        <v>186</v>
+      </c>
+      <c r="B39" s="4" t="s">
+        <v>180</v>
       </c>
       <c r="C39" t="s">
         <v>60</v>
       </c>
-      <c r="D39" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="E39" s="3" t="s">
+      <c r="D39" t="s">
+        <v>93</v>
+      </c>
+      <c r="E39" t="s">
         <v>73</v>
       </c>
       <c r="G39" t="s">
-        <v>125</v>
+        <v>201</v>
       </c>
       <c r="H39" t="s">
         <v>73</v>
@@ -1982,22 +2035,22 @@
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>132</v>
-      </c>
-      <c r="B40" s="5" t="s">
-        <v>43</v>
+        <v>187</v>
+      </c>
+      <c r="B40" s="4" t="s">
+        <v>181</v>
       </c>
       <c r="C40" t="s">
         <v>60</v>
       </c>
-      <c r="D40" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="E40" s="3" t="s">
+      <c r="D40" t="s">
+        <v>93</v>
+      </c>
+      <c r="E40" t="s">
         <v>73</v>
       </c>
       <c r="G40" t="s">
-        <v>154</v>
+        <v>202</v>
       </c>
       <c r="H40" t="s">
         <v>73</v>
@@ -2005,22 +2058,22 @@
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>151</v>
-      </c>
-      <c r="B41" s="5" t="s">
-        <v>44</v>
+        <v>144</v>
+      </c>
+      <c r="B41" s="4" t="s">
+        <v>41</v>
       </c>
       <c r="C41" t="s">
         <v>60</v>
       </c>
-      <c r="D41" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="E41" s="3" t="s">
+      <c r="D41" t="s">
+        <v>93</v>
+      </c>
+      <c r="E41" t="s">
         <v>73</v>
       </c>
       <c r="G41" t="s">
-        <v>155</v>
+        <v>196</v>
       </c>
       <c r="H41" t="s">
         <v>73</v>
@@ -2028,22 +2081,22 @@
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>152</v>
-      </c>
-      <c r="B42" s="5" t="s">
-        <v>45</v>
+        <v>188</v>
+      </c>
+      <c r="B42" s="4" t="s">
+        <v>182</v>
       </c>
       <c r="C42" t="s">
         <v>60</v>
       </c>
-      <c r="D42" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="E42" s="3" t="s">
+      <c r="D42" t="s">
+        <v>93</v>
+      </c>
+      <c r="E42" t="s">
         <v>73</v>
       </c>
       <c r="G42" t="s">
-        <v>156</v>
+        <v>197</v>
       </c>
       <c r="H42" t="s">
         <v>73</v>
@@ -2051,24 +2104,162 @@
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>153</v>
-      </c>
-      <c r="B43" s="5" t="s">
+        <v>143</v>
+      </c>
+      <c r="B43" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C43" t="s">
+        <v>60</v>
+      </c>
+      <c r="D43" t="s">
+        <v>93</v>
+      </c>
+      <c r="E43" t="s">
+        <v>73</v>
+      </c>
+      <c r="G43" t="s">
+        <v>195</v>
+      </c>
+      <c r="H43" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>145</v>
+      </c>
+      <c r="B44" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C44" t="s">
+        <v>60</v>
+      </c>
+      <c r="D44" t="s">
+        <v>93</v>
+      </c>
+      <c r="E44" t="s">
+        <v>73</v>
+      </c>
+      <c r="G44" t="s">
+        <v>194</v>
+      </c>
+      <c r="H44" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>53</v>
+      </c>
+      <c r="B45" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="C45" t="s">
+        <v>60</v>
+      </c>
+      <c r="D45" t="s">
+        <v>93</v>
+      </c>
+      <c r="E45" t="s">
+        <v>73</v>
+      </c>
+      <c r="G45" t="s">
+        <v>193</v>
+      </c>
+      <c r="H45" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
+        <v>128</v>
+      </c>
+      <c r="B46" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="C46" t="s">
+        <v>60</v>
+      </c>
+      <c r="D46" t="s">
+        <v>93</v>
+      </c>
+      <c r="E46" t="s">
+        <v>73</v>
+      </c>
+      <c r="G46" t="s">
+        <v>192</v>
+      </c>
+      <c r="H46" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
+        <v>146</v>
+      </c>
+      <c r="B47" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C47" t="s">
+        <v>60</v>
+      </c>
+      <c r="D47" t="s">
+        <v>93</v>
+      </c>
+      <c r="E47" t="s">
+        <v>73</v>
+      </c>
+      <c r="G47" t="s">
+        <v>190</v>
+      </c>
+      <c r="H47" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
+        <v>147</v>
+      </c>
+      <c r="B48" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="C48" t="s">
+        <v>60</v>
+      </c>
+      <c r="D48" t="s">
+        <v>93</v>
+      </c>
+      <c r="E48" t="s">
+        <v>73</v>
+      </c>
+      <c r="G48" t="s">
+        <v>189</v>
+      </c>
+      <c r="H48" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
+        <v>148</v>
+      </c>
+      <c r="B49" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="C43" t="s">
-        <v>60</v>
-      </c>
-      <c r="D43" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="E43" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="G43" t="s">
-        <v>123</v>
-      </c>
-      <c r="H43" t="s">
+      <c r="C49" t="s">
+        <v>60</v>
+      </c>
+      <c r="D49" t="s">
+        <v>93</v>
+      </c>
+      <c r="E49" t="s">
+        <v>73</v>
+      </c>
+      <c r="G49" t="s">
+        <v>191</v>
+      </c>
+      <c r="H49" t="s">
         <v>73</v>
       </c>
     </row>

</xml_diff>